<commit_message>
ccdi 10 input excels for phs002518
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC06_CCDI_PHS-Accession-phs003111_TumClassif-Metastatic_AssayTyp-Sequencing.xlsx
+++ b/InputFiles/CCDI/TC06_CCDI_PHS-Accession-phs003111_TumClassif-Metastatic_AssayTyp-Sequencing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\MarchBranch\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F93507-F6C9-4CEB-B5B2-8B5A3E8A44E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D46ED57-DA07-45F0-B1C0-93117DF465F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -62,51 +62,6 @@
   </si>
   <si>
     <t>FilesTab</t>
-  </si>
-  <si>
-    <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-where p.sex_at_birth IN ['Female'] and p.race in ['Asian'] and st.phs_accession in ["phs003111"]
-with st, count(p) as num_p
-MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
-with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
-ORDER BY num_cancers desc
-with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
-MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
-with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
-ORDER BY num_sites desc
-with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
-MATCH (st)&lt;-[*..5]-(fl)
-WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:radiology_file OR fl:methylation_array_file OR fl:single_cell_sequencing_file OR fl:cytogenomic_file)
-with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
-ORDER BY num_ft desc
-with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
-OPTIONAL MATCH (st)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm1:sample)
-WHERE (pcp:participant or pcp:cell_line or pcp:pdx)
-WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm1.sample_id) as num_samples_1
-OPTIONAL MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
-WHERE (cp:cell_line or cp:pdx)
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1, count(distinct sm2.sample_id) as num_samples_2
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1 + num_samples_2 as num_samples
-MATCH (st)&lt;-[*..5]-(file)
-WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
-OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
-OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
-WHERE stp.personnel_type = 'PI'
-OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
-WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
-order by st.study_id
-RETURN DISTINCT
-  st.study_short_title as `Study Short Title`,
-st.study_id as `Study ID`,
-  CASE WHEN size(cancers) &gt; 5 THEN apoc.text.join(apoc.coll.remove(cancers, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(cancers, "\n") END as `Diagnosis (Top 5)`,
-  CASE WHEN size(sites) &gt; 5 THEN apoc.text.join(apoc.coll.remove(sites, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(sites, "\n") END as `Diagnosis Anatomic Site (Top 5)`,
-  num_p as `Number of Participants`,
-  num_samples as `Number of Samples`,
-  num_files as `Number of Files`,
-  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "\n") + "\nRead More"  else apoc.text.join(file_types, "\n") END as `File Type (Top 5)`,
-  apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
-  apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
-  apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
   </si>
   <si>
     <t>TC06_CCDI_PHS-Accession-phs003111_TumClassif-Metastatic_AssayTyp-Sequencing_Neo4jData.xlsx</t>
@@ -1850,6 +1805,231 @@
 coalesce(last_vital_status, '') as `Vital Status`
 Order by participant_id</t>
   </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(st:study)
+where st.phs_accession in ['phs002518']
+optional MATCH (p)&lt;-[:of_sample]-(sm1:sample)&lt;--(cl)&lt;--(sm2:sample)
+WHERE (cl: cell_line or cl: pdx)
+optional Match (sm2)&lt;--(file)
+WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file) 
+with p, case COLLECT(distinct sm1) when [] then []
+                else COLLECT(DISTINCT {
+                        sample_anatomic_site: sm1.anatomic_site,
+                        participant_age_at_collection: sm1.participant_age_at_collection,
+                        sample_tumor_status: sm1.sample_tumor_status,
+                        tumor_classification: sm1.tumor_classification,
+                        assay_method: CASE LABELS(file)[0]
+                                  WHEN 'sequencing_file' THEN 'Sequencing'
+                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                                  WHEN 'pathology_file' THEN 'Pathology imaging'
+                                  WHEN 'methylation_array_file' THEN 'Methylation array'
+                                  ELSE null END,
+                        file_type: CASE LABELS(file)[0]
+                                  When null then null
+                                  else file.file_type end,
+                        library_selection: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_selection
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                                      ELSE null END,
+                        library_source: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_source
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
+                                      ELSE null END,
+                        library_strategy: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_strategy
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                                      ELSE null END
+                    }) end AS sample1,
+                    case COLLECT(distinct sm2) 
+                    when [] then []
+                    else COLLECT(DISTINCT {
+                        sample_anatomic_site: sm2.anatomic_site,
+                        participant_age_at_collection: sm2.participant_age_at_collection,
+                        sample_tumor_status: sm2.sample_tumor_status,
+                        tumor_classification: sm2.tumor_classification,
+                        assay_method: CASE LABELS(file)[0]
+                                  WHEN 'sequencing_file' THEN 'Sequencing'
+                                  WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                                  WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                                  WHEN 'pathology_file' THEN 'Pathology imaging'
+                                  WHEN 'methylation_array_file' THEN 'Methylation array'
+                                  ELSE null END,
+                        file_type: CASE LABELS(file)[0]
+                                  When null then null
+                                  else file.file_type end,
+                        library_selection: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_selection
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                                      ELSE null END,
+                        library_source: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_source
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_source
+                                      ELSE null END,
+                        library_strategy: CASE LABELS(file)[0]
+                                      WHEN 'sequencing_file' THEN file.library_strategy
+                                      WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                                      ELSE null END
+                    }) end AS sample2
+with p, apoc.coll.union(sample1,sample2) as cell_line_pdx_file_filters
+OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)&lt;--(file)
+WHERE (file: sequencing_file OR file:pathology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+with p, cell_line_pdx_file_filters, COLLECT(DISTINCT {
+              sample_anatomic_site: sm.anatomic_site,
+              participant_age_at_collection: sm.participant_age_at_collection,
+              sample_tumor_status: sm.sample_tumor_status,
+              tumor_classification: sm.tumor_classification,
+              assay_method: CASE LABELS(file)[0]
+                        WHEN 'sequencing_file' THEN 'Sequencing'
+                        WHEN 'single_cell_sequencing_file' THEN 'Single Cell Sequencing'
+                        WHEN 'cytogenomic_file' THEN 'Cytogenomic'
+                        WHEN 'pathology_file' THEN 'Pathology imaging'
+                        WHEN 'methylation_array_file' THEN 'Methylation array' END,
+              file_type: file.file_type,
+              library_selection: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_selection
+                            WHEN 'single_cell_sequencing_file' THEN file.library_selection
+                            ELSE null END,
+              library_source: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_source
+                              WHEN 'single_cell_sequencing_file' THEN file.library_source
+                            ELSE null END,
+              library_strategy: CASE LABELS(file)[0]
+                            WHEN 'sequencing_file' THEN file.library_strategy
+                            WHEN 'single_cell_sequencing_file' THEN file.library_strategy
+                            ELSE null END
+          }) AS general_file_filters
+OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (p)&lt;-[:of_clinical_measure_file]-(file1:clinical_measure_file)
+with p, cell_line_pdx_file_filters, general_file_filters,sm, COLLECT(DISTINCT file1.file_type) as file1_types
+UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
+with p, cell_line_pdx_file_filters, general_file_filters, COLLECT(DISTINCT {
+          sample_anatomic_site: sm.anatomic_site,
+          participant_age_at_collection: sm.participant_age_at_collection,
+          sample_tumor_status: sm.sample_tumor_status,
+          tumor_classification: sm.tumor_classification,
+          assay_method: CASE types_1 when null then null else 'Clinical data' end,
+          file_type: types_1,
+          library_selection: null,
+          library_source: null,
+          library_strategy: null
+  }) as participant_clinical_measure_file_filters
+OPTIONAL Match (p)&lt;-[:of_sample]-(sm:sample)
+OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(file1:radiology_file)
+with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, sm, COLLECT(DISTINCT file1.file_type) as file1_types
+UNWIND (case file1_types when [] then [null] else file1_types end)  AS types_1
+with p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, COLLECT(DISTINCT {
+          sample_anatomic_site: sm.anatomic_site,
+          participant_age_at_collection: sm.participant_age_at_collection,
+          sample_tumor_status: sm.sample_tumor_status,
+          tumor_classification: sm.tumor_classification,
+          assay_method: CASE types_1 when null then null else 'Radiology imaging' end,
+          file_type: types_1,
+          library_selection: null,
+          library_source: null,
+          library_strategy: null
+  }) as participant_radiology_file_filters
+OPTIONAL MATCH (p)&lt;-[*..4]-(file)
+WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
+OPTIONAL MATCH (p)&lt;-[:of_follow_up]-(fu:follow_up)
+OPTIONAL MATCH (st:study)&lt;-[:of_participant]-(p)
+OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+WITH p, cell_line_pdx_file_filters, general_file_filters, participant_clinical_measure_file_filters, participant_radiology_file_filters, file, fu, st, stf, stp, dg
+with DISTINCT
+  p.id as id,
+  p.participant_id as participant_id,
+  apoc.text.split(p.race, ';') as race,
+  p.race as race_str,
+  p.sex_at_birth as sex_at_birth,
+  p.ethnicity as ethnicity_str,
+  p.alternate_participant_id as alternate_participant_id,
+  COLLECT(DISTINCT {
+      age_at_diagnosis: dg.age_at_diagnosis,
+      diagnosis_anatomic_site: dg.anatomic_site,
+      disease_phase: dg.disease_phase,
+      diagnosis_classification_system: dg.diagnosis_classification_system,
+      diagnosis_verification_status: dg.diagnosis_verification_status,
+      diagnosis_basis: dg.diagnosis_basis,
+      diagnosis_comment: dg.diagnosis_comment,
+      diagnosis_classification: dg.diagnosis_classification
+  }) AS diagnosis_filters,
+  COLLECT(DISTINCT fu.vital_status) as vital_status,
+  apoc.coll.union(cell_line_pdx_file_filters, general_file_filters) + participant_clinical_measure_file_filters + participant_radiology_file_filters AS sample_file_filters,
+  st.study_id as study_id,
+  st.phs_accession as phs_accession,
+  COLLECT(DISTINCT stf.grant_id) as grant_id,
+  COLLECT(DISTINCT stp.institution) as institution,
+  st.study_acronym as study_acronym,
+  st.study_short_title as study_short_title
+   with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, diagnosis_filters, vital_status, sample_file_filters
+    unwind diagnosis_filters as diagnosis_filter
+  with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, diagnosis_filter, vital_status, sample_file_filters
+    with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, vital_status, sample_file_filters
+   unwind sample_file_filters as sample_file_filter
+  with id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id, sample_file_filter
+  where  sample_file_filter.tumor_classification in ['Metastatic'] and sample_file_filter.assay_method in ['Sequencing']   
+  with distinct id, participant_id, phs_accession, sex_at_birth, race_str, ethnicity_str, alternate_participant_id
+  with distinct phs_accession as study_ids
+  MATCH (st:study)&lt;-[:of_participant]-(p:participant)
+  where st.study_id = study_ids
+  with st, count(p) as num_p
+  MATCH (st:study)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
+  with st, num_p, dg.diagnosis_classification as dg_cancers, count(dg.diagnosis_classification) as num_cancers
+  ORDER BY num_cancers desc
+  with st, num_p, collect(dg_cancers + ' (' + toString(num_cancers) + ')') as cancers
+  MATCH (st)&lt;-[:of_participant]-(pa:participant)&lt;-[:of_diagnosis]-(diag:diagnosis)
+  with st, num_p, cancers, diag.anatomic_site as dg_sites, count(diag.anatomic_site) as num_sites
+  ORDER BY num_sites desc
+  with st, num_p, cancers, collect(dg_sites + ' (' + toString(num_sites) + ')') as sites
+  MATCH (st)&lt;-[*..5]-(fl)
+  WHERE (fl:clinical_measure_file OR fl: sequencing_file OR fl:pathology_file OR fl:radiology_file OR fl:methylation_array_file OR fl:single_cell_sequencing_file OR fl:cytogenomic_file)
+  with st, num_p, cancers, sites, fl.file_type as ft, count(fl.file_type) as num_ft
+  ORDER BY num_ft desc
+  with st, num_p, cancers, sites, collect(ft + ' (' + toString(num_ft) + ')') as file_types, sum(num_ft) as num_files
+  OPTIONAL MATCH (st)&lt;-[:of_participant|of_cell_line|of_pdx]-(pcp)&lt;-[:of_sample]-(sm1:sample)
+  WHERE (pcp:participant or pcp:cell_line or pcp:pdx)
+  WITH st, num_p, cancers, sites, file_types, num_files, count(distinct sm1.sample_id) as num_samples_1
+  OPTIONAL MATCH (st)&lt;-[:of_participant]-(participant)&lt;-[:of_sample]-(sm1:sample)&lt;--(cp)&lt;--(sm2:sample)
+  WHERE (cp:cell_line or cp:pdx)
+  WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1, count(distinct sm2.sample_id) as num_samples_2
+  WITH st, num_p, cancers, sites, file_types, num_files, num_samples_1 + num_samples_2 as num_samples
+  MATCH (st)&lt;-[*..5]-(file)
+  WHERE (file:clinical_measure_file OR file: sequencing_file OR file:pathology_file OR file:radiology_file OR file:methylation_array_file OR file:single_cell_sequencing_file OR file:cytogenomic_file)
+  OPTIONAL MATCH (st)&lt;-[:of_publication]-(pub:publication)
+  OPTIONAL MATCH (st)&lt;-[:of_study_personnel]-(stp:study_personnel)
+  WHERE stp.personnel_type = 'PI'
+  OPTIONAL MATCH (st)&lt;-[:of_study_funding]-(stf:study_funding)
+  WITH st, num_p, cancers, sites, file_types, num_files, num_samples, file.id as file_id, stf, stp, pub
+  with DISTINCT
+      st.id as id,
+      st.study_id as study_id,
+      apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as grant_id,
+      apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as pubmed_ids,
+      st.phs_accession as phs_accession,
+      st.study_short_title as study_short_title,
+      st.study_acronym as study_acronym,
+      apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as PIs,
+      num_p as num_of_participants,
+      cancers as diagnosis_cancer,
+      sites as diagnosis_anatomic_site,
+      file_types as file_types,
+      num_samples as num_of_samples,
+      num_files as num_of_files
+  RETURN DISTINCT
+  study_short_title as `Study Short Title`,
+  study_id as `Study ID`,
+  CASE WHEN size(diagnosis_cancer) &gt; 5 THEN apoc.text.join(apoc.coll.remove(diagnosis_cancer, 5, 10000), '\n') + '\nRead More'  else apoc.text.join(diagnosis_cancer, '\n') END as `Diagnosis (Top 5)`,
+  CASE WHEN size(diagnosis_anatomic_site) &gt; 5 THEN apoc.text.join(apoc.coll.remove(diagnosis_anatomic_site, 5, 10000), '\n') + '\nRead More'  else apoc.text.join(diagnosis_anatomic_site, '\n') END as `Diagnosis Anatomic Site (Top 5)`,
+  num_of_participants as `Number of Participants`,
+  num_of_samples as `Number of Samples`,
+  num_of_files as `Number of Files`,
+  CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), '\n') + '\nRead More'  else apoc.text.join(file_types, '\n') END as `File Type (Top 5)`,
+  pubmed_ids as `PubMed ID`,
+  PIs as `Principal Investigator(s)`,
+  grant_id as `Grant ID`</t>
+  </si>
 </sst>
 </file>
 
@@ -2235,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,16 +2450,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2287,16 +2467,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2304,16 +2484,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2321,16 +2501,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
@@ -2338,16 +2518,16 @@
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>